<commit_message>
experimented with new prompts
</commit_message>
<xml_diff>
--- a/output/prompt_experiment_Daily Energy Expenditure through the Human Life Course 2023-04-06.xlsx
+++ b/output/prompt_experiment_Daily Energy Expenditure through the Human Life Course 2023-04-06.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93345f1c83a5c894/lighthouse/Ginkgo coding/content-summarization/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6CA302AD-87A0-47CF-B517-3A44EAC99F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{6CA302AD-87A0-47CF-B517-3A44EAC99F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D85F92FB-58F7-4306-BF57-AB2C77596C5D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776"/>
+    <workbookView minimized="1" xWindow="3456" yWindow="1524" windowWidth="16608" windowHeight="15756" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prompt_experiment_Daily Energy " sheetId="1" r:id="rId1"/>
+    <sheet name="ratings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>article_title</t>
   </si>
@@ -246,11 +260,32 @@
   <si>
     <t>seniors</t>
   </si>
+  <si>
+    <t>Silvia's rating</t>
+  </si>
+  <si>
+    <t>excellent</t>
+  </si>
+  <si>
+    <t>reasonable</t>
+  </si>
+  <si>
+    <t>not quite accurate</t>
+  </si>
+  <si>
+    <t>poorly writte</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>unable to get summary</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -728,13 +763,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1090,11 +1128,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,29 +1146,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B1" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1">
         <v>4</v>
       </c>
       <c r="F1" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1256,7 +1300,7 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1291,7 +1335,7 @@
       <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1510,6 +1554,159 @@
       </c>
       <c r="I15" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64214503-9AFF-472A-8B87-7C30D7E9B0EF}">
+          <x14:formula1>
+            <xm:f>ratings!$C:$C</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:XFD1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F03790-6A70-476F-A14A-8120928048FE}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>B1</f>
+        <v>Silvia's rating</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="str">
+        <f>A2&amp;" "&amp;B2</f>
+        <v>5 excellent</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C7" si="0">A3&amp;" "&amp;B3</f>
+        <v>4 reasonable</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>3 not quite accurate</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>2 poorly writte</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>1 wrong</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>0 unable to get summary</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>